<commit_message>
WIP: Start on some long overdue corrections with an aim toward finishing this thing.
</commit_message>
<xml_diff>
--- a/Cryptography.xlsx
+++ b/Cryptography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E06A991-169D-4577-8B40-E130806AC1E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC841EC-D203-465D-842B-C1B0CC84743E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="1" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitution Ciphers" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="357">
   <si>
     <t>n = 7 (where 'n' is the prime number)</t>
   </si>
@@ -1059,18 +1059,12 @@
     <t>...</t>
   </si>
   <si>
-    <t>gcd(e, m)</t>
-  </si>
-  <si>
     <t>(e, d)</t>
   </si>
   <si>
     <t>Inverse?</t>
   </si>
   <si>
-    <t>d x e = 1 mod m</t>
-  </si>
-  <si>
     <t>(11 x 1 mod 26 = 11)</t>
   </si>
   <si>
@@ -1111,6 +1105,15 @@
   </si>
   <si>
     <t>GCD(5,  24) = 1</t>
+  </si>
+  <si>
+    <t>gcd(e, n)</t>
+  </si>
+  <si>
+    <t>d x e = 1 mod n</t>
+  </si>
+  <si>
+    <t>(11 x 19 mod 26 = 1)</t>
   </si>
 </sst>
 </file>
@@ -1665,32 +1668,32 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.28515625" customWidth="1"/>
-    <col min="22" max="22" width="65.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.109375" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.33203125" customWidth="1"/>
+    <col min="22" max="22" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R1" s="1" t="s">
         <v>93</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="14"/>
       <c r="C2" s="46" t="s">
@@ -1729,7 +1732,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="14"/>
       <c r="C3" s="45" t="s">
@@ -1768,7 +1771,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2926,7 +2929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -2983,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -3325,13 +3328,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="U31" s="48" t="s">
         <v>117</v>
       </c>
       <c r="V31" s="48"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="U32" t="s">
         <v>35</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="21:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="21:22" x14ac:dyDescent="0.3">
       <c r="U33" t="s">
         <v>36</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="21:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="21:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="U34" s="30" t="s">
         <v>37</v>
       </c>
@@ -3355,13 +3358,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="21:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="21:22" x14ac:dyDescent="0.3">
       <c r="V35" s="29"/>
     </row>
-    <row r="36" spans="21:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="21:22" x14ac:dyDescent="0.3">
       <c r="V36" s="29"/>
     </row>
-    <row r="37" spans="21:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="21:22" x14ac:dyDescent="0.3">
       <c r="V37" s="29"/>
     </row>
   </sheetData>
@@ -3389,28 +3392,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
@@ -3449,7 +3452,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3474,7 +3477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3493,7 +3496,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -3553,7 +3556,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -3572,7 +3575,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -3689,7 +3692,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>294</v>
       </c>
@@ -3700,12 +3703,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H19" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>12</v>
       </c>
@@ -3716,7 +3719,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
         <v>285</v>
       </c>
@@ -3731,31 +3734,31 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>300</v>
       </c>
@@ -3780,7 +3783,7 @@
       <c r="N1" s="33"/>
       <c r="Q1" s="33"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3799,10 +3802,10 @@
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="33" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3828,22 +3831,22 @@
         <v>302</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="R3" s="38" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3881,10 +3884,10 @@
         <v>11</v>
       </c>
       <c r="R4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3928,10 +3931,10 @@
         <v>22</v>
       </c>
       <c r="R5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3973,10 +3976,10 @@
         <v>7</v>
       </c>
       <c r="R6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4014,10 +4017,10 @@
         <v>18</v>
       </c>
       <c r="R7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4061,7 +4064,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4100,7 +4103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H11" s="4">
         <v>8</v>
       </c>
@@ -4169,7 +4172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>316</v>
       </c>
@@ -4202,7 +4205,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H13" s="4">
         <v>10</v>
       </c>
@@ -4229,7 +4232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>300</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -4336,7 +4339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>4</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>5</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>6</v>
       </c>
@@ -4445,7 +4448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>7</v>
       </c>
@@ -4475,7 +4478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>8</v>
       </c>
@@ -4502,8 +4505,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>9</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4553,7 +4559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
         <v>317</v>
       </c>
@@ -4572,7 +4578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N26" s="4">
         <v>23</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N27" s="4">
         <v>24</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N28" s="4">
         <v>25</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>300</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>1</v>
       </c>
@@ -4661,7 +4667,7 @@
       <c r="C30" s="37"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>2</v>
       </c>
@@ -4676,7 +4682,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>3</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>4</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>5</v>
       </c>
@@ -4708,7 +4714,7 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>6</v>
       </c>
@@ -4724,7 +4730,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>7</v>
       </c>
@@ -4736,7 +4742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>8</v>
       </c>
@@ -4746,7 +4752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>9</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>10</v>
       </c>
@@ -4774,7 +4780,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>11</v>
       </c>
@@ -4791,12 +4797,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="42" t="s">
         <v>318</v>
       </c>
@@ -4804,12 +4810,12 @@
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>300</v>
       </c>
@@ -4826,7 +4832,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>1</v>
       </c>
@@ -4836,7 +4842,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>2</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>3</v>
       </c>
@@ -4859,7 +4865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>4</v>
       </c>
@@ -4869,7 +4875,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>5</v>
       </c>
@@ -4879,7 +4885,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>6</v>
       </c>
@@ -4895,7 +4901,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>7</v>
       </c>
@@ -4909,7 +4915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>8</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>9</v>
       </c>
@@ -4933,13 +4939,13 @@
         <v>333</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="42" t="s">
         <v>330</v>
       </c>
@@ -4947,19 +4953,19 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E57" s="49" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F57" s="49"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>300</v>
       </c>
@@ -4973,16 +4979,16 @@
         <v>7</v>
       </c>
       <c r="E58" s="38" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F58" s="38" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G58" s="39" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>1</v>
       </c>
@@ -4994,7 +5000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>2</v>
       </c>
@@ -5006,7 +5012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>3</v>
       </c>
@@ -5022,10 +5028,10 @@
       </c>
       <c r="F61" s="4"/>
       <c r="G61" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>4</v>
       </c>
@@ -5040,7 +5046,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>5</v>
       </c>
@@ -5055,10 +5061,10 @@
         <v>121</v>
       </c>
       <c r="G63" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>6</v>
       </c>
@@ -5074,10 +5080,10 @@
       </c>
       <c r="F64" s="4"/>
       <c r="G64" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>7</v>
       </c>
@@ -5091,7 +5097,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>8</v>
       </c>
@@ -5102,7 +5108,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>9</v>
       </c>
@@ -5117,10 +5123,10 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>10</v>
       </c>
@@ -5134,7 +5140,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>11</v>
       </c>
@@ -5148,10 +5154,10 @@
         <v>21</v>
       </c>
       <c r="G69" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>12</v>
       </c>
@@ -5161,18 +5167,18 @@
         <v>3</v>
       </c>
       <c r="G70" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="42" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5193,29 +5199,29 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.109375" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="95.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>298</v>
       </c>
@@ -5226,7 +5232,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="27"/>
       <c r="C2" s="4"/>
@@ -5235,7 +5241,7 @@
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5246,7 +5252,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
@@ -5265,7 +5271,7 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>23</v>
       </c>
@@ -5291,7 +5297,7 @@
       <c r="I5" s="49"/>
       <c r="J5" s="49"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -5333,7 +5339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -5372,7 +5378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8" s="32">
         <f>LCM(A7-1,B7-1)</f>
         <v>12</v>
@@ -5399,7 +5405,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>124</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
@@ -5458,7 +5464,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>126</v>
       </c>
@@ -5482,7 +5488,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
@@ -5513,7 +5519,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -5543,7 +5549,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>128</v>
       </c>
@@ -5567,7 +5573,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -5586,7 +5592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -5612,7 +5618,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -5638,7 +5644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>131</v>
       </c>
@@ -5660,7 +5666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
@@ -5691,7 +5697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
@@ -5715,7 +5721,7 @@
       </c>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>134</v>
       </c>
@@ -5741,7 +5747,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5760,7 +5766,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
@@ -5787,7 +5793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>36</v>
       </c>
@@ -5808,7 +5814,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>37</v>
       </c>
@@ -5830,7 +5836,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>141</v>
       </c>
@@ -5846,7 +5852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
@@ -5865,7 +5871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>36</v>
       </c>
@@ -5884,7 +5890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>37</v>
       </c>
@@ -5903,7 +5909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>320</v>
       </c>
@@ -5919,7 +5925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>27</v>
       </c>
@@ -5951,59 +5957,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="15:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="15:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="O33" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="C61" s="24"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="2"/>
     </row>
@@ -6023,30 +6029,30 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="47" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" customWidth="1"/>
-    <col min="20" max="25" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="20" max="25" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J1" s="49" t="s">
         <v>114</v>
       </c>
@@ -6056,7 +6062,7 @@
       </c>
       <c r="M1" s="49"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>107</v>
       </c>
@@ -6079,7 +6085,7 @@
       <c r="Q2" s="49"/>
       <c r="R2" s="49"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -6134,26 +6140,26 @@
       <c r="T3" s="48"/>
       <c r="U3" s="48"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
       <c r="C4">
         <f>A4*B4</f>
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f>INDEX(P5:P53,MATCH(1,Q5:Q53,0))</f>
         <v>5</v>
       </c>
       <c r="F4">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
         <v>63</v>
@@ -6194,17 +6200,17 @@
       </c>
       <c r="U4" s="29"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="D5">
         <f>(A4-1)*(B4-1)</f>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <f>INDEX(P4:P53,MATCH(1,R4:R53,0))</f>
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
         <v>64</v>
@@ -6245,13 +6251,13 @@
       </c>
       <c r="U5" s="29"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="D6">
         <f>LCM(A4-1,B4-1)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <f>MOD(F5,D4)</f>
@@ -6269,19 +6275,19 @@
       </c>
       <c r="K6" s="13">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L6" s="26">
         <f t="shared" si="2"/>
-        <v>4.4601490397061246E+43</v>
-      </c>
-      <c r="M6" s="31" t="e">
+        <v>4194304</v>
+      </c>
+      <c r="M6" s="31">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N6" t="e">
+        <v>2</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P6">
         <v>3</v>
@@ -6296,7 +6302,7 @@
       </c>
       <c r="U6" s="29"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6312,26 +6318,26 @@
       </c>
       <c r="K7" s="13">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="L7" s="26">
         <f t="shared" si="2"/>
-        <v>1.088690056823018E+44</v>
-      </c>
-      <c r="M7" s="13" t="e">
+        <v>48828125</v>
+      </c>
+      <c r="M7" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N7" t="e">
+        <v>3</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P7">
         <v>4</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R7" s="7" t="str">
         <f t="shared" si="5"/>
@@ -6339,7 +6345,7 @@
       </c>
       <c r="U7" s="29"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6355,19 +6361,19 @@
       </c>
       <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L8" s="26">
         <f t="shared" si="2"/>
-        <v>4.7101286972462449E+27</v>
-      </c>
-      <c r="M8" s="13" t="e">
+        <v>2048</v>
+      </c>
+      <c r="M8" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N8" t="e">
+        <v>4</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P8">
         <v>5</v>
@@ -6382,7 +6388,7 @@
       </c>
       <c r="U8" s="29"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -6398,19 +6404,19 @@
       </c>
       <c r="K9" s="13">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L9" s="26">
         <f t="shared" si="2"/>
-        <v>9.9999999999999991E+28</v>
-      </c>
-      <c r="M9" s="13" t="e">
+        <v>177147</v>
+      </c>
+      <c r="M9" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N9" t="e">
+        <v>5</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P9">
         <v>6</v>
@@ -6421,11 +6427,11 @@
       </c>
       <c r="R9" s="7">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U9" s="29"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>13</v>
       </c>
@@ -6445,15 +6451,15 @@
       </c>
       <c r="L10" s="26">
         <f t="shared" si="2"/>
-        <v>3.6845653286788893E+22</v>
-      </c>
-      <c r="M10" s="13" t="e">
+        <v>362797056</v>
+      </c>
+      <c r="M10" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N10" t="e">
+        <v>6</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P10">
         <v>7</v>
@@ -6464,11 +6470,11 @@
       </c>
       <c r="R10" s="7">
         <f>IF(P10&lt;=E$4,"-",MOD(P10*E$4,D$4))</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="U10" s="29"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>17</v>
       </c>
@@ -6488,30 +6494,30 @@
       </c>
       <c r="L11" s="26">
         <f t="shared" si="2"/>
-        <v>3.2199057558131799E+24</v>
-      </c>
-      <c r="M11" s="13" t="e">
+        <v>1977326743</v>
+      </c>
+      <c r="M11" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" t="e">
+        <v>7</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P11">
         <v>8</v>
       </c>
       <c r="Q11">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R11" s="7">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="U11" s="29"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>19</v>
       </c>
@@ -6531,15 +6537,15 @@
       </c>
       <c r="L12" s="26">
         <f t="shared" si="2"/>
-        <v>1.5474250491067253E+26</v>
-      </c>
-      <c r="M12" s="13" t="e">
+        <v>8589934592</v>
+      </c>
+      <c r="M12" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" t="e">
+        <v>8</v>
+      </c>
+      <c r="N12" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P12">
         <v>9</v>
@@ -6550,11 +6556,11 @@
       </c>
       <c r="R12" s="7">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="U12" s="29"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H13" t="s">
         <v>72</v>
       </c>
@@ -6567,19 +6573,19 @@
       </c>
       <c r="K13" s="13">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="L13" s="26">
         <f t="shared" si="2"/>
-        <v>2.8823037615171174E+17</v>
-      </c>
-      <c r="M13" s="13" t="e">
+        <v>285311670611</v>
+      </c>
+      <c r="M13" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N13" t="e">
+        <v>9</v>
+      </c>
+      <c r="N13" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P13">
         <v>10</v>
@@ -6594,7 +6600,7 @@
       </c>
       <c r="U13" s="29"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
         <v>73</v>
       </c>
@@ -6607,19 +6613,19 @@
       </c>
       <c r="K14" s="13">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L14" s="26">
         <f t="shared" si="2"/>
-        <v>1.8626451492309569E+20</v>
-      </c>
-      <c r="M14" s="13" t="e">
+        <v>743008370688</v>
+      </c>
+      <c r="M14" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" t="e">
+        <v>10</v>
+      </c>
+      <c r="N14" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P14">
         <v>11</v>
@@ -6630,11 +6636,11 @@
       </c>
       <c r="R14" s="7">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U14" s="29"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
         <v>74</v>
       </c>
@@ -6647,34 +6653,34 @@
       </c>
       <c r="K15" s="13">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L15" s="26">
         <f t="shared" si="2"/>
-        <v>8.3076749736557242E+34</v>
-      </c>
-      <c r="M15" s="13" t="e">
+        <v>31381059609</v>
+      </c>
+      <c r="M15" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N15" t="e">
+        <v>11</v>
+      </c>
+      <c r="N15" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P15">
         <v>12</v>
       </c>
       <c r="Q15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="U15" s="29"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H16" t="s">
         <v>75</v>
       </c>
@@ -6687,19 +6693,19 @@
       </c>
       <c r="K16" s="13">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="L16" s="26">
         <f t="shared" si="2"/>
-        <v>4.8196857210675092E+35</v>
-      </c>
-      <c r="M16" s="13" t="e">
+        <v>100000000000</v>
+      </c>
+      <c r="M16" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N16" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P16">
         <v>13</v>
@@ -6710,11 +6716,11 @@
       </c>
       <c r="R16" s="7">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="U16" s="29"/>
     </row>
-    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
         <v>76</v>
       </c>
@@ -6731,15 +6737,15 @@
       </c>
       <c r="L17" s="26">
         <f t="shared" si="2"/>
-        <v>2.0153812643461118E+32</v>
-      </c>
-      <c r="M17" s="13" t="e">
+        <v>1792160394037</v>
+      </c>
+      <c r="M17" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N17" t="e">
+        <v>13</v>
+      </c>
+      <c r="N17" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>yes</v>
       </c>
       <c r="P17">
         <v>14</v>
@@ -6750,11 +6756,11 @@
       </c>
       <c r="R17" s="7">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="U17" s="29"/>
     </row>
-    <row r="18" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H18" t="s">
         <v>77</v>
       </c>
@@ -6767,19 +6773,19 @@
       </c>
       <c r="K18" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L18" s="26">
         <f>POWER(K18,F$4)</f>
-        <v>1.7286737396774712E+33</v>
-      </c>
-      <c r="M18" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N18" t="e">
+        <v>0</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P18">
         <v>15</v>
@@ -6794,7 +6800,7 @@
       </c>
       <c r="U18" s="29"/>
     </row>
-    <row r="19" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
         <v>78</v>
       </c>
@@ -6807,34 +6813,34 @@
       </c>
       <c r="K19" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="L19" s="26">
         <f t="shared" si="2"/>
-        <v>1.2783403948858939E+34</v>
-      </c>
-      <c r="M19" s="13" t="e">
+        <v>1</v>
+      </c>
+      <c r="M19" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N19" t="e">
+        <v>1</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P19">
         <v>16</v>
       </c>
       <c r="Q19">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R19" s="7">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="U19" s="29"/>
     </row>
-    <row r="20" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
         <v>79</v>
       </c>
@@ -6847,19 +6853,19 @@
       </c>
       <c r="K20" s="13">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L20" s="26">
         <f t="shared" si="2"/>
-        <v>1.5863092971714916E+30</v>
-      </c>
-      <c r="M20" s="13" t="e">
+        <v>4194304</v>
+      </c>
+      <c r="M20" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N20" t="e">
+        <v>2</v>
+      </c>
+      <c r="N20" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P20">
         <v>17</v>
@@ -6870,11 +6876,11 @@
       </c>
       <c r="R20" s="7">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="U20" s="29"/>
     </row>
-    <row r="21" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
         <v>80</v>
       </c>
@@ -6887,19 +6893,19 @@
       </c>
       <c r="K21" s="13">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L21" s="26">
         <f t="shared" si="2"/>
-        <v>1.9781359483314151E+31</v>
-      </c>
-      <c r="M21" s="13" t="e">
+        <v>48828125</v>
+      </c>
+      <c r="M21" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N21" t="e">
+        <v>3</v>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P21">
         <v>18</v>
@@ -6910,11 +6916,11 @@
       </c>
       <c r="R21" s="7">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="U21" s="29"/>
     </row>
-    <row r="22" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H22" t="s">
         <v>81</v>
       </c>
@@ -6927,19 +6933,19 @@
       </c>
       <c r="K22" s="13">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="L22" s="26">
         <f t="shared" si="2"/>
-        <v>3.0910586430935376E+39</v>
-      </c>
-      <c r="M22" s="13" t="e">
+        <v>2048</v>
+      </c>
+      <c r="M22" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N22" t="e">
+        <v>4</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P22">
         <v>19</v>
@@ -6950,10 +6956,10 @@
       </c>
       <c r="R22" s="7">
         <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="8:21" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H23" t="s">
         <v>82</v>
       </c>
@@ -6966,33 +6972,33 @@
       </c>
       <c r="K23" s="13">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="L23" s="26">
         <f t="shared" si="2"/>
-        <v>1.0620036506406717E+40</v>
-      </c>
-      <c r="M23" s="13" t="e">
+        <v>177147</v>
+      </c>
+      <c r="M23" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N23" t="e">
+        <v>5</v>
+      </c>
+      <c r="N23" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P23">
         <v>20</v>
       </c>
       <c r="Q23">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H24" t="s">
         <v>83</v>
       </c>
@@ -7005,19 +7011,19 @@
       </c>
       <c r="K24" s="13">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L24" s="26">
         <f t="shared" si="2"/>
-        <v>5.3687091199999995E+37</v>
-      </c>
-      <c r="M24" s="13" t="e">
+        <v>362797056</v>
+      </c>
+      <c r="M24" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N24" t="e">
+        <v>6</v>
+      </c>
+      <c r="N24" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P24">
         <v>21</v>
@@ -7028,10 +7034,10 @@
       </c>
       <c r="R24" s="7">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="8:21" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H25" t="s">
         <v>84</v>
       </c>
@@ -7044,19 +7050,19 @@
       </c>
       <c r="K25" s="13">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="L25" s="26">
         <f t="shared" si="2"/>
-        <v>2.2098334710081732E+38</v>
-      </c>
-      <c r="M25" s="13" t="e">
+        <v>1977326743</v>
+      </c>
+      <c r="M25" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N25" t="e">
+        <v>7</v>
+      </c>
+      <c r="N25" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P25">
         <v>22</v>
@@ -7067,10 +7073,10 @@
       </c>
       <c r="R25" s="7">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="8:21" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>85</v>
       </c>
@@ -7083,19 +7089,19 @@
       </c>
       <c r="K26" s="13">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="L26" s="26">
         <f t="shared" si="2"/>
-        <v>8.5164331908653772E+38</v>
-      </c>
-      <c r="M26" s="13" t="e">
+        <v>8589934592</v>
+      </c>
+      <c r="M26" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N26" t="e">
+        <v>8</v>
+      </c>
+      <c r="N26" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P26">
         <v>23</v>
@@ -7106,10 +7112,10 @@
       </c>
       <c r="R26" s="7">
         <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="8:21" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
         <v>86</v>
       </c>
@@ -7122,33 +7128,33 @@
       </c>
       <c r="K27" s="13">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="L27" s="26">
         <f t="shared" si="2"/>
-        <v>2.5287310893279634E+36</v>
-      </c>
-      <c r="M27" s="13" t="e">
+        <v>285311670611</v>
+      </c>
+      <c r="M27" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N27" t="e">
+        <v>9</v>
+      </c>
+      <c r="N27" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P27">
         <v>24</v>
       </c>
       <c r="Q27">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="R27" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
         <v>87</v>
       </c>
@@ -7161,19 +7167,19 @@
       </c>
       <c r="K28" s="13">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="L28" s="26">
         <f t="shared" si="2"/>
-        <v>1.2129821994589221E+37</v>
-      </c>
-      <c r="M28" s="13" t="e">
+        <v>743008370688</v>
+      </c>
+      <c r="M28" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N28" t="e">
+        <v>10</v>
+      </c>
+      <c r="N28" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P28">
         <v>25</v>
@@ -7187,7 +7193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H29" t="s">
         <v>88</v>
       </c>
@@ -7200,19 +7206,19 @@
       </c>
       <c r="K29" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L29" s="26">
         <f t="shared" si="2"/>
-        <v>6.8630377364882997E+42</v>
-      </c>
-      <c r="M29" s="13" t="e">
+        <v>31381059609</v>
+      </c>
+      <c r="M29" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N29" t="e">
+        <v>11</v>
+      </c>
+      <c r="N29" t="str">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>no</v>
       </c>
       <c r="P29">
         <v>26</v>
@@ -7223,10 +7229,10 @@
       </c>
       <c r="R29" s="7">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="8:21" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="8:21" x14ac:dyDescent="0.3">
       <c r="P30">
         <v>27</v>
       </c>
@@ -7236,23 +7242,23 @@
       </c>
       <c r="R30" s="7">
         <f t="shared" ref="R30:R35" si="8">IF(P30&lt;=E$4,"-",MOD(P30*E$4,D$4))</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="8:21" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="8:21" x14ac:dyDescent="0.3">
       <c r="P31">
         <v>28</v>
       </c>
       <c r="Q31">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="8:21" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="8:21" x14ac:dyDescent="0.3">
       <c r="P32">
         <v>29</v>
       </c>
@@ -7265,7 +7271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P33">
         <v>30</v>
       </c>
@@ -7275,10 +7281,10 @@
       </c>
       <c r="R33" s="7">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="16:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P34">
         <v>31</v>
       </c>
@@ -7288,23 +7294,23 @@
       </c>
       <c r="R34" s="7">
         <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="16:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P35">
         <v>32</v>
       </c>
       <c r="Q35">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R35" s="7">
         <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="16:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P36">
         <v>33</v>
       </c>
@@ -7314,10 +7320,10 @@
       </c>
       <c r="R36" s="7">
         <f t="shared" ref="R36:R53" si="10">IF(P36&lt;=E$4,"-",MOD(P36*E$4,D$4))</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="16:18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P37">
         <v>34</v>
       </c>
@@ -7330,7 +7336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P38">
         <v>35</v>
       </c>
@@ -7340,23 +7346,23 @@
       </c>
       <c r="R38" s="7">
         <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="16:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P39">
         <v>36</v>
       </c>
       <c r="Q39">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R39" s="7">
         <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="16:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P40">
         <v>37</v>
       </c>
@@ -7366,10 +7372,10 @@
       </c>
       <c r="R40" s="7">
         <f t="shared" si="10"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="16:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P41">
         <v>38</v>
       </c>
@@ -7379,10 +7385,10 @@
       </c>
       <c r="R41" s="7">
         <f t="shared" si="10"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="16:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P42">
         <v>39</v>
       </c>
@@ -7395,20 +7401,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P43">
         <v>40</v>
       </c>
       <c r="Q43">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R43" s="7">
         <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="16:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P44">
         <v>41</v>
       </c>
@@ -7418,10 +7424,10 @@
       </c>
       <c r="R44" s="7">
         <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="16:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P45">
         <v>42</v>
       </c>
@@ -7431,10 +7437,10 @@
       </c>
       <c r="R45" s="7">
         <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="16:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P46">
         <v>43</v>
       </c>
@@ -7444,23 +7450,23 @@
       </c>
       <c r="R46" s="7">
         <f t="shared" si="10"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="16:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P47">
         <v>44</v>
       </c>
       <c r="Q47">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R47" s="7">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P48">
         <v>45</v>
       </c>
@@ -7470,10 +7476,10 @@
       </c>
       <c r="R48" s="7">
         <f t="shared" si="10"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="16:18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P49">
         <v>46</v>
       </c>
@@ -7483,10 +7489,10 @@
       </c>
       <c r="R49" s="7">
         <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="16:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P50">
         <v>47</v>
       </c>
@@ -7496,23 +7502,23 @@
       </c>
       <c r="R50" s="7">
         <f t="shared" si="10"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="16:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P51">
         <v>48</v>
       </c>
       <c r="Q51">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="R51" s="7">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P52">
         <v>49</v>
       </c>
@@ -7525,7 +7531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="16:18" x14ac:dyDescent="0.3">
       <c r="P53">
         <v>50</v>
       </c>
@@ -7535,7 +7541,7 @@
       </c>
       <c r="R53" s="7">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7573,19 +7579,19 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>185</v>
       </c>
@@ -7606,7 +7612,7 @@
       </c>
       <c r="H1" s="34"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>159</v>
       </c>
@@ -7623,7 +7629,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -7640,7 +7646,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -7657,7 +7663,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -7674,7 +7680,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>167</v>
       </c>
@@ -7691,7 +7697,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -7711,7 +7717,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -7728,7 +7734,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -7745,7 +7751,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>174</v>
       </c>
@@ -7753,7 +7759,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>175</v>
       </c>
@@ -7764,7 +7770,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -7773,13 +7779,13 @@
       </c>
       <c r="H12" s="29"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>179</v>
       </c>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>180</v>
       </c>
@@ -7788,7 +7794,7 @@
       </c>
       <c r="H14" s="29"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>182</v>
       </c>
@@ -7797,7 +7803,7 @@
       </c>
       <c r="H15" s="29"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -7812,13 +7818,13 @@
       </c>
       <c r="H16" s="29"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>187</v>
       </c>
       <c r="H17" s="29"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>67</v>
       </c>
@@ -7830,7 +7836,7 @@
       </c>
       <c r="H18" s="29"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -7839,7 +7845,7 @@
       </c>
       <c r="H19" s="29"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>78</v>
       </c>
@@ -7848,7 +7854,7 @@
       </c>
       <c r="H20" s="29"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>181</v>
       </c>
@@ -7860,13 +7866,13 @@
       </c>
       <c r="H21" s="29"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>194</v>
       </c>
       <c r="H22" s="29"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>209</v>
       </c>
@@ -7881,7 +7887,7 @@
       </c>
       <c r="H23" s="29"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>196</v>
       </c>
@@ -7896,7 +7902,7 @@
       </c>
       <c r="H24" s="29"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -7907,7 +7913,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>202</v>
       </c>
@@ -7921,12 +7927,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -7934,7 +7940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -7942,7 +7948,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>208</v>
       </c>
@@ -7950,7 +7956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -7958,7 +7964,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>196</v>
       </c>
@@ -7966,7 +7972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>202</v>
       </c>
@@ -7988,19 +7994,19 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>231</v>
       </c>
@@ -8011,7 +8017,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>230</v>
       </c>
@@ -8022,7 +8028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -8033,7 +8039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -8044,7 +8050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -8055,7 +8061,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -8069,7 +8075,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>232</v>
       </c>
@@ -8083,7 +8089,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>254</v>
       </c>
@@ -8109,7 +8115,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -8132,7 +8138,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>245</v>
       </c>
@@ -8155,7 +8161,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -8166,7 +8172,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>256</v>
       </c>
@@ -8180,7 +8186,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>255</v>
       </c>
@@ -8203,7 +8209,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>262</v>
       </c>
@@ -8223,7 +8229,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>263</v>
       </c>
@@ -8247,7 +8253,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -8272,17 +8278,17 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -8296,7 +8302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8320,7 +8326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D4">
         <f>D3-B3</f>
         <v>-3</v>
@@ -8334,7 +8340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H5" s="26">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -8344,7 +8350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H6" s="26">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -8354,7 +8360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H7" s="26">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -8364,7 +8370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H8" s="26">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -8374,7 +8380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H9" s="26">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -8384,7 +8390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H10" s="26">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -8394,7 +8400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H11" s="26">
         <f t="shared" ref="H11:H40" si="2">H10+H$3</f>
         <v>18</v>
@@ -8404,7 +8410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="26">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -8414,7 +8420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H13" s="26">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -8424,7 +8430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H14" s="26">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -8434,7 +8440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" s="26">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -8444,7 +8450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" s="26">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -8454,7 +8460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="26">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -8464,7 +8470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="26">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -8474,7 +8480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="26">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -8484,7 +8490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="26">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -8494,7 +8500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="26">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -8504,7 +8510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="26">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8514,7 +8520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="26">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8524,7 +8530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="26">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8534,7 +8540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="26">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -8544,7 +8550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="26">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -8554,7 +8560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="26">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -8564,7 +8570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="26">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -8574,7 +8580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="26">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -8584,7 +8590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="26">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -8594,7 +8600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="26">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -8604,7 +8610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="26">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -8614,7 +8620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="26">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -8624,7 +8630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="26">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -8634,7 +8640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="26">
         <f t="shared" si="2"/>
         <v>66</v>
@@ -8644,7 +8650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36" s="26">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -8654,7 +8660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37" s="26">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -8664,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38" s="26">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -8674,7 +8680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="26">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -8684,7 +8690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H40" s="26">
         <f t="shared" si="2"/>
         <v>76</v>

</xml_diff>

<commit_message>
WIP: More updates...getting closer.
</commit_message>
<xml_diff>
--- a/Cryptography.xlsx
+++ b/Cryptography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265D58E0-60CC-4CFC-A9CD-8BECB7295FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F7D5F-8468-40F2-BCEB-5C6CC780DD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitution Ciphers" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="375">
   <si>
     <t>n = 7 (where 'n' is the prime number)</t>
   </si>
@@ -1153,6 +1153,15 @@
   </si>
   <si>
     <t>gcd(5, 24) = 1</t>
+  </si>
+  <si>
+    <t>(4 ^ 29 = 9 mod 35)</t>
+  </si>
+  <si>
+    <t>(9 ^ 5 = 4 mod 35)</t>
+  </si>
+  <si>
+    <t>Figure 10. Digital signing.</t>
   </si>
 </sst>
 </file>
@@ -3778,20 +3787,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E13DE6-8DF4-4B7C-B600-DC44B025BC54}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" customWidth="1"/>
     <col min="8" max="8" width="8.109375" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
@@ -6391,12 +6400,159 @@
         <v>340</v>
       </c>
     </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E74" s="52"/>
+      <c r="F74" s="52"/>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F75" s="38"/>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
+        <v>1</v>
+      </c>
+      <c r="B76" s="46">
+        <v>4</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
+        <v>2</v>
+      </c>
+      <c r="B77" s="4">
+        <v>9</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" t="s">
+        <v>372</v>
+      </c>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" s="4">
+        <v>3</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="37">
+        <v>9</v>
+      </c>
+      <c r="D78" s="4">
+        <v>9</v>
+      </c>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
+        <v>4</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="46">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>373</v>
+      </c>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B80" s="4"/>
+      <c r="C80" s="37"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="37"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="46"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S4:S29">
     <sortCondition ref="S4:S29"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E74:F74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrections/clarifications in sections dealing with DH.
</commit_message>
<xml_diff>
--- a/Cryptography.xlsx
+++ b/Cryptography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F7D5F-8468-40F2-BCEB-5C6CC780DD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19898333-1591-4A1B-9E23-7024168C00E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitution Ciphers" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="374">
   <si>
     <t>n = 7 (where 'n' is the prime number)</t>
   </si>
@@ -969,9 +969,6 @@
     <t>(3,7)</t>
   </si>
   <si>
-    <t>(3 ^ 3 mod 7 = 6)</t>
-  </si>
-  <si>
     <t>Exponent</t>
   </si>
   <si>
@@ -1032,12 +1029,6 @@
     <t>Figure 6. Finding the modular multiplicative inverse.</t>
   </si>
   <si>
-    <t>(3 ^ 1 mod 7 = 3)</t>
-  </si>
-  <si>
-    <t>(3 ^ 2 mod 7 = 2)</t>
-  </si>
-  <si>
     <t>...</t>
   </si>
   <si>
@@ -1162,6 +1153,12 @@
   </si>
   <si>
     <t>Figure 10. Digital signing.</t>
+  </si>
+  <si>
+    <t>(3 ^ 1 = 3 mod 7)</t>
+  </si>
+  <si>
+    <t>(3 ^ 2 = 2 mod 7)</t>
   </si>
 </sst>
 </file>
@@ -3789,16 +3786,16 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.44140625" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="6" max="6" width="7.88671875" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" customWidth="1"/>
@@ -3859,11 +3856,11 @@
         <v>96</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="33" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
@@ -3880,28 +3877,28 @@
         <v>2</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>312</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>302</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="R3" s="39" t="s">
         <v>302</v>
@@ -3914,10 +3911,10 @@
       </c>
       <c r="V3" s="45"/>
       <c r="W3" s="45" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
@@ -3941,7 +3938,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>331</v>
+        <v>372</v>
       </c>
       <c r="N4" s="5">
         <v>1</v>
@@ -3958,22 +3955,22 @@
         <v>11</v>
       </c>
       <c r="R4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="W4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="Y4" s="39" t="s">
         <v>302</v>
@@ -4006,7 +4003,7 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>332</v>
+        <v>373</v>
       </c>
       <c r="N5" s="4">
         <v>2</v>
@@ -4023,7 +4020,7 @@
         <v>22</v>
       </c>
       <c r="R5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="T5" s="5">
         <v>1</v>
@@ -4043,7 +4040,7 @@
         <v>5</v>
       </c>
       <c r="Y5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
@@ -4071,7 +4068,7 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="N6" s="5">
         <v>3</v>
@@ -4088,7 +4085,7 @@
         <v>7</v>
       </c>
       <c r="R6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="T6" s="4">
         <v>2</v>
@@ -4108,7 +4105,7 @@
         <v>10</v>
       </c>
       <c r="Y6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
@@ -4132,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="N7" s="4">
         <v>4</v>
@@ -4149,7 +4146,7 @@
         <v>18</v>
       </c>
       <c r="R7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="T7" s="5">
         <v>3</v>
@@ -4169,7 +4166,7 @@
         <v>15</v>
       </c>
       <c r="Y7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
@@ -4213,7 +4210,7 @@
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="T8" s="4">
         <v>4</v>
@@ -4233,7 +4230,7 @@
         <v>20</v>
       </c>
       <c r="Y8" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
@@ -4292,7 +4289,7 @@
         <v>1</v>
       </c>
       <c r="Y9" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
@@ -4354,7 +4351,7 @@
         <v>6</v>
       </c>
       <c r="Y10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -4401,12 +4398,12 @@
         <v>11</v>
       </c>
       <c r="Y11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -4666,7 +4663,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="H17" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N17" s="4">
         <v>14</v>
@@ -4908,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="T22" s="4">
         <v>18</v>
@@ -5014,7 +5011,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N25" s="4">
         <v>22</v>
@@ -5234,7 +5231,7 @@
       </c>
       <c r="D31" s="4"/>
       <c r="N31" s="42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T31" s="4">
         <v>27</v>
@@ -5314,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="Y33" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
@@ -5333,10 +5330,10 @@
         <v>3</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="R34" s="25"/>
       <c r="T34" s="4">
@@ -5370,7 +5367,7 @@
       </c>
       <c r="D35" s="4"/>
       <c r="E35" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="N35" s="5">
         <v>1</v>
@@ -5501,7 +5498,7 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="N38" s="5">
         <v>4</v>
@@ -5592,7 +5589,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="N40" s="4">
         <v>6</v>
@@ -5628,14 +5625,14 @@
         <v>No</v>
       </c>
       <c r="T41" s="47" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="U41" s="47"/>
       <c r="V41" s="47"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -5760,7 +5757,7 @@
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D47" s="4">
         <v>11</v>
@@ -5840,7 +5837,7 @@
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="N50" s="5">
         <v>16</v>
@@ -5920,7 +5917,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="N53" s="5">
         <v>19</v>
@@ -5959,7 +5956,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -6001,7 +5998,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E57" s="52" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F57" s="52"/>
       <c r="N57" s="5">
@@ -6033,10 +6030,10 @@
         <v>7</v>
       </c>
       <c r="E58" s="38" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F58" s="38" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G58" s="39" t="s">
         <v>302</v>
@@ -6124,7 +6121,7 @@
       </c>
       <c r="F61" s="4"/>
       <c r="G61" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N61" s="5">
         <v>27</v>
@@ -6183,7 +6180,7 @@
         <v>121</v>
       </c>
       <c r="G63" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="N63" s="5">
         <v>29</v>
@@ -6215,7 +6212,7 @@
       </c>
       <c r="F64" s="4"/>
       <c r="G64" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="N64" s="4">
         <v>30</v>
@@ -6299,7 +6296,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N67" s="5">
         <v>33</v>
@@ -6357,7 +6354,7 @@
         <v>21</v>
       </c>
       <c r="G69" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="N69" s="5">
         <v>35</v>
@@ -6383,7 +6380,7 @@
       </c>
       <c r="C70" s="4"/>
       <c r="G70" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
@@ -6392,12 +6389,12 @@
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="N71" s="47" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="42" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
@@ -6445,7 +6442,7 @@
       </c>
       <c r="D77" s="4"/>
       <c r="E77" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F77" s="4"/>
     </row>
@@ -6472,7 +6469,7 @@
         <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F79" s="4"/>
     </row>
@@ -6484,7 +6481,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="47" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="37"/>
@@ -6792,10 +6789,10 @@
         <v>32</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>28</v>
@@ -6848,10 +6845,10 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -6873,16 +6870,16 @@
         <v>6</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -6912,7 +6909,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -6931,12 +6928,12 @@
         <v>4</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -7277,7 +7274,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H30">
         <v>25</v>
@@ -7296,7 +7293,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H31">
         <v>26</v>

</xml_diff>

<commit_message>
Add equations to RSA.
</commit_message>
<xml_diff>
--- a/Cryptography.xlsx
+++ b/Cryptography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDDD3B-5004-4342-92AB-2F6AB9A552B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88259A9-097A-4F0F-B3F5-98048FCF32FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="7" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitution Ciphers" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="539">
   <si>
     <t>n = 7 (where 'n' is the prime number)</t>
   </si>
@@ -1056,9 +1056,6 @@
     <t>(3 x 11 = 7 mod 26)</t>
   </si>
   <si>
-    <t>gcd(5, 24) = 1</t>
-  </si>
-  <si>
     <t>(4 ^ 29 = 9 mod 35)</t>
   </si>
   <si>
@@ -1197,9 +1194,6 @@
     <t>Proof of correctness</t>
   </si>
   <si>
-    <t>Integers</t>
-  </si>
-  <si>
     <t>e x d = 1 mod n</t>
   </si>
   <si>
@@ -1209,9 +1203,6 @@
     <t>gcd(e,n)</t>
   </si>
   <si>
-    <t>e x d = 1 mod t</t>
-  </si>
-  <si>
     <t>Hash of message</t>
   </si>
   <si>
@@ -1648,6 +1639,21 @@
   </si>
   <si>
     <t>(13,7)</t>
+  </si>
+  <si>
+    <t>(5,35)</t>
+  </si>
+  <si>
+    <t>(e,n)</t>
+  </si>
+  <si>
+    <t>gcd(5,24) = 1</t>
+  </si>
+  <si>
+    <t>gcd(e,t(n))</t>
+  </si>
+  <si>
+    <t>e x d = 1 mod t(n)</t>
   </si>
 </sst>
 </file>
@@ -4291,39 +4297,38 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E13DE6-8DF4-4B7C-B600-DC44B025BC54}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y145"/>
+  <dimension ref="A1:X145"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.6640625" customWidth="1"/>
-    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>276</v>
       </c>
@@ -4348,7 +4353,7 @@
       <c r="N1" s="33"/>
       <c r="Q1" s="33"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4360,7 +4365,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="N2" s="33" t="s">
-        <v>386</v>
+        <v>96</v>
       </c>
       <c r="O2" s="33" t="s">
         <v>329</v>
@@ -4372,7 +4377,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4398,22 +4403,22 @@
         <v>278</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="R3" s="39" t="s">
         <v>278</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>386</v>
+        <v>286</v>
       </c>
       <c r="U3" s="45" t="s">
         <v>25</v>
@@ -4422,13 +4427,10 @@
         <v>316</v>
       </c>
       <c r="W3" s="45" t="s">
-        <v>329</v>
-      </c>
-      <c r="X3" s="45" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N4" s="5">
         <v>1</v>
@@ -4469,25 +4471,22 @@
         <v>324</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="U4" s="9" t="s">
         <v>315</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>143</v>
+        <v>537</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="Y4" s="39" t="s">
+        <v>538</v>
+      </c>
+      <c r="X4" s="39" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4514,7 +4513,7 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N5" s="4">
         <v>2</v>
@@ -4543,18 +4542,15 @@
         <f>GCD(T5,U5)</f>
         <v>1</v>
       </c>
-      <c r="W5" s="5">
-        <v>35</v>
-      </c>
-      <c r="X5" s="4">
-        <f t="shared" ref="X5:X39" si="4">MOD(T5*T$9,U5)</f>
+      <c r="W5" s="4">
+        <f t="shared" ref="W5:W39" si="4">MOD(T5*T$9,U5)</f>
         <v>5</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="X5" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4608,18 +4604,15 @@
         <f t="shared" ref="V6:V39" si="5">GCD(T6,U6)</f>
         <v>2</v>
       </c>
-      <c r="W6" s="5">
-        <v>35</v>
-      </c>
-      <c r="X6" s="4">
+      <c r="W6" s="4">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="X6" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4669,18 +4662,15 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W7" s="5">
-        <v>35</v>
-      </c>
-      <c r="X7" s="4">
+      <c r="W7" s="4">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="X7" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4733,18 +4723,15 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="W8" s="5">
-        <v>35</v>
-      </c>
-      <c r="X8" s="4">
+      <c r="W8" s="4">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="X8" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4792,18 +4779,15 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W9" s="5">
-        <v>35</v>
-      </c>
-      <c r="X9" s="4">
+      <c r="W9" s="4">
         <f>MOD(T9*T$9,U9)</f>
         <v>1</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="X9" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4854,18 +4838,15 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="W10" s="5">
-        <v>35</v>
-      </c>
-      <c r="X10" s="4">
+      <c r="W10" s="4">
         <f>MOD(T10*T$9,U10)</f>
         <v>6</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="X10" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="H11" s="4">
         <v>8</v>
       </c>
@@ -4901,18 +4882,15 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W11" s="5">
-        <v>35</v>
-      </c>
-      <c r="X11" s="4">
+      <c r="W11" s="4">
         <f>MOD(T11*T$9,U11)</f>
         <v>11</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="X11" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>289</v>
       </c>
@@ -4954,15 +4932,12 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="W12" s="5">
-        <v>35</v>
-      </c>
-      <c r="X12" s="4">
+      <c r="W12" s="4">
         <f>MOD(T12*T$9,U12)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="H13" s="4">
         <v>10</v>
       </c>
@@ -4998,15 +4973,12 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W13" s="5">
-        <v>35</v>
-      </c>
-      <c r="X13" s="4">
+      <c r="W13" s="4">
         <f>MOD(T13*T$9,U13)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>276</v>
       </c>
@@ -5057,15 +5029,12 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W14" s="5">
-        <v>35</v>
-      </c>
-      <c r="X14" s="4">
+      <c r="W14" s="4">
         <f>MOD(T14*T$9,U14)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -5111,15 +5080,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W15" s="5">
-        <v>35</v>
-      </c>
-      <c r="X15" s="4">
+      <c r="W15" s="4">
         <f>MOD(T15*T$9,U15)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -5156,15 +5122,12 @@
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="W16" s="5">
-        <v>35</v>
-      </c>
-      <c r="X16" s="4">
+      <c r="W16" s="4">
         <f>MOD(T16*T$9,U16)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
@@ -5200,15 +5163,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W17" s="5">
-        <v>35</v>
-      </c>
-      <c r="X17" s="4">
+      <c r="W17" s="4">
         <f>MOD(T17*T$9,U17)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>4</v>
       </c>
@@ -5247,15 +5207,12 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W18" s="5">
-        <v>35</v>
-      </c>
-      <c r="X18" s="4">
+      <c r="W18" s="4">
         <f>MOD(T18*T$9,U18)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>5</v>
       </c>
@@ -5292,15 +5249,12 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W19" s="5">
-        <v>35</v>
-      </c>
-      <c r="X19" s="4">
+      <c r="W19" s="4">
         <f>MOD(T19*T$9,U19)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>6</v>
       </c>
@@ -5333,15 +5287,12 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="W20" s="5">
-        <v>35</v>
-      </c>
-      <c r="X20" s="4">
+      <c r="W20" s="4">
         <f>MOD(T20*T$9,U20)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>7</v>
       </c>
@@ -5380,15 +5331,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W21" s="5">
-        <v>35</v>
-      </c>
-      <c r="X21" s="4">
+      <c r="W21" s="4">
         <f>MOD(T21*T$9,U21)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>8</v>
       </c>
@@ -5428,15 +5376,12 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="W22" s="5">
-        <v>35</v>
-      </c>
-      <c r="X22" s="4">
+      <c r="W22" s="4">
         <f>MOD(T22*T$9,U22)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>9</v>
       </c>
@@ -5476,15 +5421,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W23" s="5">
-        <v>35</v>
-      </c>
-      <c r="X23" s="4">
+      <c r="W23" s="4">
         <f>MOD(T23*T$9,U23)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -5512,15 +5454,12 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="W24" s="5">
-        <v>35</v>
-      </c>
-      <c r="X24" s="4">
+      <c r="W24" s="4">
         <f>MOD(T24*T$9,U24)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
         <v>290</v>
       </c>
@@ -5548,15 +5487,12 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W25" s="5">
-        <v>35</v>
-      </c>
-      <c r="X25" s="4">
+      <c r="W25" s="4">
         <f>MOD(T25*T$9,U25)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N26" s="4">
         <v>23</v>
       </c>
@@ -5581,15 +5517,12 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W26" s="5">
-        <v>35</v>
-      </c>
-      <c r="X26" s="4">
+      <c r="W26" s="4">
         <f>MOD(T26*T$9,U26)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N27" s="4">
         <v>24</v>
       </c>
@@ -5614,15 +5547,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W27" s="5">
-        <v>35</v>
-      </c>
-      <c r="X27" s="4">
+      <c r="W27" s="4">
         <f>MOD(T27*T$9,U27)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N28" s="4">
         <v>25</v>
       </c>
@@ -5647,15 +5577,12 @@
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="W28" s="5">
-        <v>35</v>
-      </c>
-      <c r="X28" s="4">
+      <c r="W28" s="4">
         <f>MOD(T28*T$9,U28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>276</v>
       </c>
@@ -5695,15 +5622,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W29" s="5">
-        <v>35</v>
-      </c>
-      <c r="X29" s="4">
+      <c r="W29" s="4">
         <f>MOD(T29*T$9,U29)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>1</v>
       </c>
@@ -5722,15 +5646,12 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W30" s="5">
-        <v>35</v>
-      </c>
-      <c r="X30" s="4">
+      <c r="W30" s="4">
         <f>MOD(T30*T$9,U30)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>2</v>
       </c>
@@ -5754,15 +5675,12 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W31" s="5">
-        <v>35</v>
-      </c>
-      <c r="X31" s="4">
+      <c r="W31" s="4">
         <f>MOD(T31*T$9,U31)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>3</v>
       </c>
@@ -5783,15 +5701,12 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="W32" s="5">
-        <v>35</v>
-      </c>
-      <c r="X32" s="4">
+      <c r="W32" s="4">
         <f>MOD(T32*T$9,U32)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>4</v>
       </c>
@@ -5814,18 +5729,15 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W33" s="5">
-        <v>35</v>
-      </c>
-      <c r="X33" s="43">
+      <c r="W33" s="43">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="X33" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>5</v>
       </c>
@@ -5855,15 +5767,12 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="W34" s="5">
-        <v>35</v>
-      </c>
-      <c r="X34" s="4">
+      <c r="W34" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>6</v>
       </c>
@@ -5899,15 +5808,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W35" s="5">
-        <v>35</v>
-      </c>
-      <c r="X35" s="4">
+      <c r="W35" s="4">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>7</v>
       </c>
@@ -5939,15 +5845,12 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="W36" s="5">
-        <v>35</v>
-      </c>
-      <c r="X36" s="4">
+      <c r="W36" s="4">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>8</v>
       </c>
@@ -5977,15 +5880,12 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="W37" s="5">
-        <v>35</v>
-      </c>
-      <c r="X37" s="4">
+      <c r="W37" s="4">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>9</v>
       </c>
@@ -6021,15 +5921,12 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="W38" s="5">
-        <v>35</v>
-      </c>
-      <c r="X38" s="4">
+      <c r="W38" s="4">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>10</v>
       </c>
@@ -6061,15 +5958,12 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W39" s="5">
-        <v>35</v>
-      </c>
-      <c r="X39" s="4">
+      <c r="W39" s="4">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>11</v>
       </c>
@@ -6097,7 +5991,7 @@
       </c>
       <c r="Q40" s="4"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -6118,7 +6012,7 @@
       <c r="U41" s="47"/>
       <c r="V41" s="47"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="42" t="s">
         <v>291</v>
       </c>
@@ -6137,7 +6031,7 @@
       </c>
       <c r="Q42" s="4"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -6153,7 +6047,7 @@
       </c>
       <c r="Q43" s="4"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>276</v>
       </c>
@@ -6181,7 +6075,7 @@
       </c>
       <c r="Q44" s="4"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>1</v>
       </c>
@@ -6202,7 +6096,7 @@
       </c>
       <c r="Q45" s="4"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>2</v>
       </c>
@@ -6224,7 +6118,7 @@
       </c>
       <c r="Q46" s="4"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>3</v>
       </c>
@@ -6247,7 +6141,7 @@
       </c>
       <c r="Q47" s="4"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>4</v>
       </c>
@@ -6544,9 +6438,7 @@
         <f>B59*B60</f>
         <v>35</v>
       </c>
-      <c r="C61" s="37" t="s">
-        <v>275</v>
-      </c>
+      <c r="C61" s="37"/>
       <c r="E61" s="4" t="s">
         <v>3</v>
       </c>
@@ -6570,15 +6462,18 @@
       <c r="A62" s="4">
         <v>4</v>
       </c>
-      <c r="C62" s="4">
-        <f>B61</f>
-        <v>35</v>
-      </c>
-      <c r="D62" s="4">
-        <v>35</v>
-      </c>
+      <c r="B62" s="4">
+        <f>(B59-1)*(B60-1)</f>
+        <v>24</v>
+      </c>
+      <c r="C62" s="37"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="G62" t="s">
+        <v>313</v>
+      </c>
       <c r="N62" s="4">
         <v>28</v>
       </c>
@@ -6596,16 +6491,17 @@
         <v>5</v>
       </c>
       <c r="B63" s="4">
-        <f>(B59-1)*(B60-1)</f>
-        <v>24</v>
-      </c>
-      <c r="C63" s="37"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>121</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="4"/>
       <c r="G63" t="s">
-        <v>313</v>
+        <v>536</v>
       </c>
       <c r="N63" s="51">
         <v>29</v>
@@ -6623,19 +6519,16 @@
       <c r="A64" s="4">
         <v>6</v>
       </c>
-      <c r="B64" s="4">
+      <c r="C64" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="D64" s="4">
         <v>5</v>
       </c>
-      <c r="C64" s="37" t="s">
-        <v>275</v>
-      </c>
       <c r="E64" s="4" t="s">
-        <v>20</v>
+        <v>535</v>
       </c>
       <c r="F64" s="4"/>
-      <c r="G64" t="s">
-        <v>339</v>
-      </c>
       <c r="N64" s="4">
         <v>30</v>
       </c>
@@ -6653,11 +6546,9 @@
         <v>7</v>
       </c>
       <c r="B65" s="4"/>
-      <c r="C65" s="4">
-        <v>5</v>
-      </c>
+      <c r="C65" s="37"/>
       <c r="D65" s="4">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -6789,11 +6680,8 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
       <c r="N71" s="47" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
@@ -6846,7 +6734,7 @@
       </c>
       <c r="D77" s="4"/>
       <c r="E77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F77" s="4"/>
     </row>
@@ -6873,7 +6761,7 @@
         <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F79" s="4"/>
     </row>
@@ -6885,7 +6773,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="47" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="37"/>
@@ -6930,7 +6818,7 @@
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F84" s="4"/>
     </row>
@@ -6945,7 +6833,7 @@
         <v>2</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -6958,7 +6846,7 @@
       <c r="C86" s="37"/>
       <c r="D86" s="4"/>
       <c r="E86" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F86" s="4"/>
     </row>
@@ -6975,7 +6863,7 @@
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F87" s="4"/>
     </row>
@@ -6990,7 +6878,7 @@
         <v>6</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -7002,7 +6890,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -7016,7 +6904,7 @@
         <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -7027,7 +6915,7 @@
         <v>5</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -7039,7 +6927,7 @@
         <v>24</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -7055,7 +6943,7 @@
         <v>29</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -7063,11 +6951,11 @@
         <v>11</v>
       </c>
       <c r="C94" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -7080,7 +6968,7 @@
       <c r="C95" s="37"/>
       <c r="D95" s="4"/>
       <c r="E95" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -7093,7 +6981,7 @@
       <c r="C96" s="37"/>
       <c r="D96" s="4"/>
       <c r="E96" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -7107,7 +6995,7 @@
       <c r="C97" s="37"/>
       <c r="D97" s="4"/>
       <c r="E97" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -7119,7 +7007,7 @@
         <v>5</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -7131,13 +7019,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="47" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="37"/>
       <c r="D100" s="4"/>
       <c r="E100" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -7209,7 +7097,7 @@
         <v>57</v>
       </c>
       <c r="F105" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -7225,10 +7113,10 @@
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F106" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -7257,7 +7145,7 @@
         <v>56</v>
       </c>
       <c r="F108" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -7270,10 +7158,10 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F109" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -7287,7 +7175,7 @@
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -7303,10 +7191,10 @@
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F111" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -7315,14 +7203,14 @@
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D112" s="4">
         <f>B110</f>
         <v>5</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -7350,7 +7238,7 @@
         <v>5</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -7364,7 +7252,7 @@
         <v>2</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -7378,7 +7266,7 @@
         <v>6</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -7392,7 +7280,7 @@
         <v>true</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -7404,13 +7292,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="47" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -7479,10 +7367,10 @@
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F124" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -7498,10 +7386,10 @@
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F125" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -7525,10 +7413,10 @@
         <v>4</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F127" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -7542,7 +7430,7 @@
         <v>201</v>
       </c>
       <c r="F128" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -7554,10 +7442,10 @@
         <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F129" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -7571,10 +7459,10 @@
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F130" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -7593,7 +7481,7 @@
         <v>201</v>
       </c>
       <c r="F131" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -7607,10 +7495,10 @@
         <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F132" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -7627,7 +7515,7 @@
         <v>149</v>
       </c>
       <c r="F133" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -7641,10 +7529,10 @@
         <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F134" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -7658,10 +7546,10 @@
         <v>Verified</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F135" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -7672,10 +7560,10 @@
       <c r="C136" s="4"/>
       <c r="D136" s="52"/>
       <c r="E136" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F136" t="s">
         <v>400</v>
-      </c>
-      <c r="F136" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -7686,10 +7574,10 @@
       <c r="C137" s="4"/>
       <c r="D137" s="52"/>
       <c r="E137" s="53" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F137" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -7700,10 +7588,10 @@
       <c r="C138" s="4"/>
       <c r="D138" s="52"/>
       <c r="E138" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F138" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -7714,10 +7602,10 @@
       <c r="C139" s="4"/>
       <c r="D139" s="52"/>
       <c r="E139" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F139" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -7728,10 +7616,10 @@
       <c r="C140" s="4"/>
       <c r="D140" s="52"/>
       <c r="E140" s="3" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F140" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -7741,10 +7629,10 @@
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="E141" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F141" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -7762,7 +7650,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="47" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -7771,12 +7659,12 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="X9:X32">
-    <sortCondition ref="X9:X32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="W9:W32">
+    <sortCondition ref="W9:W32"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="E57:F57"/>
@@ -10583,8 +10471,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10606,7 +10494,7 @@
         <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -10650,7 +10538,7 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -10661,7 +10549,7 @@
         <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D6" t="s">
         <v>150</v>
@@ -10675,7 +10563,7 @@
         <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D7" t="s">
         <v>230</v>
@@ -10689,7 +10577,7 @@
         <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D8" t="s">
         <v>231</v>
@@ -10708,13 +10596,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B9" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C9" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D9" t="s">
         <v>233</v>
@@ -10733,13 +10621,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C10" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D10" t="s">
         <v>235</v>
@@ -10764,7 +10652,7 @@
         <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D11" t="s">
         <v>237</v>
@@ -10778,7 +10666,7 @@
         <v>238</v>
       </c>
       <c r="C12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D12" t="s">
         <v>239</v>
@@ -10792,7 +10680,7 @@
         <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D13" t="s">
         <v>243</v>
@@ -10811,19 +10699,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B14" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D14" t="s">
         <v>245</v>
       </c>
       <c r="E14" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G14">
         <f>4-(6+5)</f>
@@ -10836,13 +10724,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B15" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C15" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D15" t="s">
         <v>246</v>
@@ -10867,7 +10755,7 @@
         <v>238</v>
       </c>
       <c r="C16" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D16" t="s">
         <v>248</v>
@@ -10878,13 +10766,13 @@
         <v>242</v>
       </c>
       <c r="B17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C17" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -10895,13 +10783,13 @@
         <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D18" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G18">
         <f>5*7</f>
@@ -10914,19 +10802,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B19" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C19" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E19" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="G19">
         <f>1-(10+5)</f>
@@ -10939,19 +10827,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D20" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G20">
         <f>10-3-6</f>
@@ -10967,16 +10855,16 @@
         <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C21" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D21" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="J21" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -10984,16 +10872,16 @@
         <v>242</v>
       </c>
       <c r="B22" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C22" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D22" t="s">
+        <v>416</v>
+      </c>
+      <c r="J22" t="s">
         <v>419</v>
-      </c>
-      <c r="J22" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -11004,13 +10892,13 @@
         <v>149</v>
       </c>
       <c r="C23" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D23" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E23" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -11020,24 +10908,24 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C24" t="s">
+        <v>463</v>
+      </c>
+      <c r="D24" t="s">
+        <v>469</v>
+      </c>
+      <c r="E24" t="s">
         <v>468</v>
-      </c>
-      <c r="C24" t="s">
-        <v>466</v>
-      </c>
-      <c r="D24" t="s">
-        <v>472</v>
-      </c>
-      <c r="E24" t="s">
-        <v>471</v>
       </c>
       <c r="G24">
         <f>0-(3+5)</f>
@@ -11048,24 +10936,24 @@
         <v>9</v>
       </c>
       <c r="J24" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B25" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C25" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D25" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E25" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G25">
         <f>0-0-1</f>
@@ -11076,7 +10964,7 @@
         <v>16</v>
       </c>
       <c r="J25" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -11084,16 +10972,16 @@
         <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C26" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D26" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J26" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -11101,16 +10989,16 @@
         <v>242</v>
       </c>
       <c r="B27" t="s">
+        <v>478</v>
+      </c>
+      <c r="C27" t="s">
         <v>481</v>
       </c>
-      <c r="C27" t="s">
-        <v>484</v>
-      </c>
       <c r="D27" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J27" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -11121,13 +11009,13 @@
         <v>149</v>
       </c>
       <c r="C28" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D28" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E28" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G28">
         <f>15*13</f>
@@ -11138,24 +11026,24 @@
         <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B29" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C29" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D29" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E29" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="G29">
         <f>64-(9+5)</f>
@@ -11166,24 +11054,24 @@
         <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B30" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C30" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D30" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E30" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G30">
         <f>72-128-16</f>
@@ -11194,7 +11082,7 @@
         <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -11202,16 +11090,16 @@
         <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C31" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D31" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="J31" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -11219,16 +11107,16 @@
         <v>242</v>
       </c>
       <c r="B32" t="s">
+        <v>493</v>
+      </c>
+      <c r="C32" t="s">
+        <v>495</v>
+      </c>
+      <c r="D32" t="s">
         <v>496</v>
       </c>
-      <c r="C32" t="s">
-        <v>498</v>
-      </c>
-      <c r="D32" t="s">
-        <v>499</v>
-      </c>
       <c r="J32" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -11239,13 +11127,13 @@
         <v>149</v>
       </c>
       <c r="C33" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D33" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G33">
         <f>12*14</f>
@@ -11256,24 +11144,24 @@
         <v>15</v>
       </c>
       <c r="J33" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B34" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C34" t="s">
+        <v>508</v>
+      </c>
+      <c r="D34" t="s">
+        <v>510</v>
+      </c>
+      <c r="E34" t="s">
         <v>511</v>
-      </c>
-      <c r="D34" t="s">
-        <v>513</v>
-      </c>
-      <c r="E34" t="s">
-        <v>514</v>
       </c>
       <c r="G34">
         <f>225-(16+5)</f>
@@ -11284,24 +11172,24 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B35" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C35" t="s">
+        <v>509</v>
+      </c>
+      <c r="D35" t="s">
         <v>512</v>
       </c>
-      <c r="D35" t="s">
-        <v>515</v>
-      </c>
       <c r="E35" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="G35">
         <f>240-0-13</f>
@@ -11312,7 +11200,7 @@
         <v>6</v>
       </c>
       <c r="J35" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -11320,13 +11208,13 @@
         <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C36" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D36" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -11334,13 +11222,13 @@
         <v>242</v>
       </c>
       <c r="B37" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C37" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D37" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -11351,13 +11239,13 @@
         <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D38" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E38" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G38">
         <f>5*10</f>
@@ -11370,19 +11258,19 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B39" t="s">
+        <v>524</v>
+      </c>
+      <c r="C39" t="s">
+        <v>526</v>
+      </c>
+      <c r="D39" t="s">
         <v>527</v>
       </c>
-      <c r="C39" t="s">
-        <v>529</v>
-      </c>
-      <c r="D39" t="s">
-        <v>530</v>
-      </c>
       <c r="E39" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="G39">
         <f>256-5</f>
@@ -11395,19 +11283,19 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B40" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C40" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D40" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E40" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="G40">
         <f>0-208-6</f>
@@ -11423,13 +11311,13 @@
         <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C41" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D41" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -11442,7 +11330,9 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11470,396 +11360,396 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <f>MOD(A3,B3)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <f>MATCH(1,I3:I40,0)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H3" s="26">
         <f>A3</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I3" s="26">
         <f t="shared" ref="I3:I40" si="0">MOD(H3,B$3)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H4" s="26">
         <f t="shared" ref="H4:H10" si="1">H3+H$3</f>
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="I4" s="26">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H5" s="26">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="I5" s="26">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H6" s="26">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="I6" s="26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H7" s="26">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="I7" s="26">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H8" s="26">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="I8" s="26">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H9" s="26">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="I9" s="26">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H10" s="26">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="I10" s="26">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H11" s="26">
         <f t="shared" ref="H11:H40" si="2">H10+H$3</f>
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="I11" s="26">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="26">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="I12" s="26">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H13" s="26">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>143</v>
       </c>
       <c r="I13" s="26">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H14" s="26">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="I14" s="26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" s="26">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>169</v>
       </c>
       <c r="I15" s="26">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" s="26">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="I16" s="26">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="26">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="I17" s="26">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="26">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>208</v>
       </c>
       <c r="I18" s="26">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="26">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>221</v>
       </c>
       <c r="I19" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="26">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>234</v>
       </c>
       <c r="I20" s="26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="26">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>247</v>
       </c>
       <c r="I21" s="26">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="26">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>260</v>
       </c>
       <c r="I22" s="26">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="26">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>273</v>
       </c>
       <c r="I23" s="26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="26">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>286</v>
       </c>
       <c r="I24" s="26">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="26">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>299</v>
       </c>
       <c r="I25" s="26">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="26">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>312</v>
       </c>
       <c r="I26" s="26">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="26">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="I27" s="26">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="26">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>338</v>
       </c>
       <c r="I28" s="26">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="26">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>351</v>
       </c>
       <c r="I29" s="26">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="26">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>364</v>
       </c>
       <c r="I30" s="26">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="26">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>377</v>
       </c>
       <c r="I31" s="26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="26">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>390</v>
       </c>
       <c r="I32" s="26">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H33" s="26">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>403</v>
       </c>
       <c r="I33" s="26">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H34" s="26">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>416</v>
       </c>
       <c r="I34" s="26">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H35" s="26">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>429</v>
       </c>
       <c r="I35" s="26">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H36" s="26">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>442</v>
       </c>
       <c r="I36" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H37" s="26">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>455</v>
       </c>
       <c r="I37" s="26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H38" s="26">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>468</v>
       </c>
       <c r="I38" s="26">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H39" s="26">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>481</v>
       </c>
       <c r="I39" s="26">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H40" s="26">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>494</v>
       </c>
       <c r="I40" s="26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add proof for RSA encryption.
</commit_message>
<xml_diff>
--- a/Cryptography.xlsx
+++ b/Cryptography.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD97AA32-F801-49EB-BE84-958F4A71BA96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0F40F3-B03A-4C57-845C-5211BF756C9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="1" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitution Ciphers" sheetId="3" r:id="rId1"/>
     <sheet name="Diffie-Hellman Key Derivation" sheetId="1" r:id="rId2"/>
     <sheet name="Figures" sheetId="11" r:id="rId3"/>
-    <sheet name="RSA" sheetId="2" r:id="rId4"/>
-    <sheet name="RSA Example" sheetId="4" r:id="rId5"/>
-    <sheet name="Elliptic Curve DH" sheetId="7" r:id="rId6"/>
-    <sheet name="EC Example" sheetId="8" r:id="rId7"/>
-    <sheet name="MMI Calculator" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
+    <sheet name="RSA" sheetId="2" r:id="rId5"/>
+    <sheet name="RSA Example" sheetId="4" r:id="rId6"/>
+    <sheet name="Elliptic Curve DH" sheetId="7" r:id="rId7"/>
+    <sheet name="EC Example" sheetId="8" r:id="rId8"/>
+    <sheet name="MMI Calculator" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Primes">'RSA Example'!$A$5:$A$12</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="542">
   <si>
     <t>n = 7 (where 'n' is the prime number)</t>
   </si>
@@ -1661,6 +1662,9 @@
   </si>
   <si>
     <t>s = ke^-1(h(m) + r*ka)</t>
+  </si>
+  <si>
+    <t>a-b</t>
   </si>
 </sst>
 </file>
@@ -3964,7 +3968,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -4306,8 +4310,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:X147"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView showGridLines="0" topLeftCell="A121" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7715,6 +7719,792 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CE62CC-EF82-4EB4-A697-0044799F4B7A}">
+  <dimension ref="A1:Q36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>B2*B1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B4">
+        <f>(B1-1)*(B2-1)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <f>MOD(A7,B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <f>MOD(POWER($A7,2),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <f>MOD(POWER($A7,3),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <f>MOD(POWER($A7,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f>MOD(POWER($A7,5),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f>MOD(POWER($A7,6),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <f>MOD(POWER($A7,7),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <f>MOD(POWER($A7,8),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <f>MOD(POWER($A7,9),$B$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <f>MOD(A8,B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C21" si="0">MOD(POWER($A8,2),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <f>MOD(POWER($A8,3),$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <f>MOD(POWER($A8,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <f>MOD(POWER($A8,5),$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <f>MOD(POWER($A8,6),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <f>MOD(POWER($A8,7),$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8:I21" si="1">MOD(POWER($A8,8),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8:J21" si="2">MOD(POWER($A8,9),$B$3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <f>MOD(A9,B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="2">
+        <f>MOD(POWER($A9,3),$B$3)</f>
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <f>MOD(POWER($A9,4),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="F9" s="2">
+        <f>MOD(POWER($A9,5),$B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <f>MOD(POWER($A9,6),$B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
+        <f>MOD(POWER($A9,7),$B$3)</f>
+        <v>12</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <f>MOD(A10,B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <f>MOD(POWER($A10,3),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <f>MOD(POWER($A10,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <f>MOD(POWER($A10,5),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="2">
+        <f>MOD(POWER($A10,6),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" ref="H10:H21" si="3">MOD(POWER($A10,7),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <f>MOD(A11,B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <f>MOD(POWER($A11,3),$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <f>MOD(POWER($A11,4),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <f>MOD(POWER($A11,5),$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <f>MOD(POWER($A11,6),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <f>MOD(A12,B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D12" s="2">
+        <f>MOD(POWER($A12,3),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <f>MOD(POWER($A12,4),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
+        <f>MOD(POWER($A12,5),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="G12" s="2">
+        <f>MOD(POWER($A12,6),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <f>MOD(A13,B$3)</f>
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <f>MOD(POWER($A13,3),$B$3)</f>
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <f>MOD(POWER($A13,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>MOD(POWER($A13,5),$B$3)</f>
+        <v>7</v>
+      </c>
+      <c r="G13" s="2">
+        <f>MOD(POWER($A13,6),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2">
+        <f>MOD(A14,B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D14" s="2">
+        <f>MOD(POWER($A14,3),$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <f>MOD(POWER($A14,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <f>MOD(POWER($A14,5),$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="G14" s="2">
+        <f>MOD(POWER($A14,6),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2">
+        <f>MOD(A15,B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D15" s="2">
+        <f>MOD(POWER($A15,3),$B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <f>MOD(POWER($A15,4),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="F15" s="2">
+        <f>MOD(POWER($A15,5),$B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
+        <f>MOD(POWER($A15,6),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <f>MOD(A16,B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
+        <f>MOD(POWER($A16,3),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
+        <f>MOD(POWER($A16,4),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <f>MOD(POWER($A16,5),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <f>MOD(POWER($A16,6),$B$3)</f>
+        <v>10</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2">
+        <f>MOD(A17,B$3)</f>
+        <v>11</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <f>MOD(POWER($A17,3),$B$3)</f>
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <f>MOD(POWER($A17,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <f>MOD(POWER($A17,5),$B$3)</f>
+        <v>11</v>
+      </c>
+      <c r="G17" s="2">
+        <f>MOD(POWER($A17,6),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2">
+        <f>MOD(A18,B$3)</f>
+        <v>12</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D18" s="2">
+        <f>MOD(POWER($A18,3),$B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <f>MOD(POWER($A18,4),$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
+        <f>MOD(POWER($A18,5),$B$3)</f>
+        <v>12</v>
+      </c>
+      <c r="G18" s="2">
+        <f>MOD(POWER($A18,6),$B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2">
+        <f>MOD(A19,B$3)</f>
+        <v>13</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <f>MOD(POWER($A19,3),$B$3)</f>
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <f>MOD(POWER($A19,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <f>MOD(POWER($A19,5),$B$3)</f>
+        <v>13</v>
+      </c>
+      <c r="G19" s="2">
+        <f>MOD(POWER($A19,6),$B$3)</f>
+        <v>4</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P19" s="15"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2">
+        <f>MOD(A20,B$3)</f>
+        <v>14</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <f>MOD(POWER($A20,3),$B$3)</f>
+        <v>14</v>
+      </c>
+      <c r="E20" s="2">
+        <f>MOD(POWER($A20,4),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <f>MOD(POWER($A20,5),$B$3)</f>
+        <v>14</v>
+      </c>
+      <c r="G20" s="2">
+        <f>MOD(POWER($A20,6),$B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P20" s="15"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2">
+        <f>MOD(A21,B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <f>MOD(POWER($A21,3),$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <f>MOD(POWER($A21,4),$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <f>MOD(POWER($A21,5),$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f>MOD(POWER($A21,6),$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="15"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>541</v>
+      </c>
+      <c r="E28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29">
+        <v>96</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <f>B29-C29</f>
+        <v>84</v>
+      </c>
+      <c r="E29">
+        <f>D29/B1</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30">
+        <v>47</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <f>B30-C30</f>
+        <v>35</v>
+      </c>
+      <c r="E30">
+        <f>D30/B2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D9BD01-0E4D-488A-9F8B-3FC9D4746A54}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O64"/>
@@ -8544,7 +9334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CA44E2-1AB0-4DBC-8381-995D301099FD}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:U53"/>
@@ -10090,7 +10880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C647415D-CFD1-4745-A53D-5DF4C6FC6939}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H33"/>
@@ -10505,7 +11295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A96A00-B420-4A12-AD77-4AD839B24B7B}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J41"/>
@@ -11364,7 +12154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E485E03-FDA4-40E5-9DDA-BB586457AA05}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I69"/>

</xml_diff>